<commit_message>
Improve workout logging UX and sync exercise list
</commit_message>
<xml_diff>
--- a/Comprehensive Exercise.xlsx
+++ b/Comprehensive Exercise.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="163">
   <si>
     <t>Body Part</t>
   </si>
@@ -64,7 +64,19 @@
     <t>Incline Dumbbeell Chest Press</t>
   </si>
   <si>
-    <t>Dumbells, Bench</t>
+    <t>Dumbells, Incline Bench</t>
+  </si>
+  <si>
+    <t>Incline Chest Press Machine</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Chest Press Machine</t>
+  </si>
+  <si>
+    <t>Plate Loaded Chest Press</t>
   </si>
   <si>
     <t>Dips</t>
@@ -82,12 +94,15 @@
     <t>Cable Machine</t>
   </si>
   <si>
+    <t>High-to-Low Cable Fly</t>
+  </si>
+  <si>
+    <t>Low-to-High Cable Fly</t>
+  </si>
+  <si>
     <t>Pec Deck</t>
   </si>
   <si>
-    <t>Machine</t>
-  </si>
-  <si>
     <t>Dumbbell Pullover</t>
   </si>
   <si>
@@ -157,6 +172,9 @@
     <t>Mid-Back / Lats</t>
   </si>
   <si>
+    <t>Cable Wide Row</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lat Pulldown </t>
   </si>
   <si>
@@ -178,7 +196,13 @@
     <t>Barbell Shrug</t>
   </si>
   <si>
-    <t>Upper Traps</t>
+    <t>Traps</t>
+  </si>
+  <si>
+    <t>Dumbbell Shrugs</t>
+  </si>
+  <si>
+    <t>Dumbbell</t>
   </si>
   <si>
     <t>Shoulders</t>
@@ -241,7 +265,7 @@
     <t>Quads</t>
   </si>
   <si>
-    <t>Back Squat (High/Low Bar)</t>
+    <t>Barbell Squat</t>
   </si>
   <si>
     <t>Overall Leg Mass</t>
@@ -259,15 +283,12 @@
     <t>Leg Press</t>
   </si>
   <si>
-    <t>Quads (Heavy Load)</t>
+    <t xml:space="preserve">Quads </t>
   </si>
   <si>
     <t>Hack Squat</t>
   </si>
   <si>
-    <t>Quads (Outer Sweep)</t>
-  </si>
-  <si>
     <t>Bulgarian Split Squat</t>
   </si>
   <si>
@@ -439,22 +460,22 @@
     <t>Peak / Isolation</t>
   </si>
   <si>
-    <t>Dumbbell</t>
-  </si>
-  <si>
     <t>Abs/Core</t>
   </si>
   <si>
     <t>Hanging Leg Raise</t>
   </si>
   <si>
-    <t>Lower Abs</t>
+    <t>Abs</t>
   </si>
   <si>
     <t>Cable Crunch</t>
   </si>
   <si>
-    <t>Upper Abs</t>
+    <t>Decline Crunch</t>
+  </si>
+  <si>
+    <t>Decline Bench</t>
   </si>
   <si>
     <t>Ab Wheel Rollout</t>
@@ -837,10 +858,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -848,13 +869,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -862,13 +883,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -876,13 +897,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
@@ -890,727 +911,839 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>107</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>113</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>128</v>
-      </c>
       <c r="D51" s="1" t="s">
-        <v>126</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>33</v>
+        <v>120</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="D62" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="1" t="s">
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add forearm support and refine muscle mask assets
</commit_message>
<xml_diff>
--- a/Comprehensive Exercise.xlsx
+++ b/Comprehensive Exercise.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="167">
   <si>
     <t>Body Part</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>Peak / Isolation</t>
+  </si>
+  <si>
+    <t>Forearms</t>
+  </si>
+  <si>
+    <t>Reverse Bar Bicep Curl</t>
+  </si>
+  <si>
+    <t>Dumbbell Forearm Curl</t>
+  </si>
+  <si>
+    <t>Cable Forearm Curl</t>
   </si>
   <si>
     <t>Abs/Core</t>
@@ -1670,10 +1682,10 @@
         <v>150</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66">
@@ -1681,13 +1693,13 @@
         <v>149</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67">
@@ -1695,38 +1707,38 @@
         <v>149</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>154</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="D68" s="1" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>26</v>
@@ -1734,16 +1746,58 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D70" s="1" t="s">
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>162</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>